<commit_message>
Added checkout information test case
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/DataFile.xlsx
+++ b/src/test/resources/TestData/DataFile.xlsx
@@ -3,12 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24326"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4F69975-66AC-44D9-B77F-8A43B528848F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A59A6954-EE42-4BF6-859E-CAEE0B95231A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="8" r:id="rId1"/>
+    <sheet name="UserInfo" sheetId="9" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Password</t>
   </si>
@@ -38,6 +39,27 @@
   </si>
   <si>
     <t>secret_sauce</t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>ZIPCode</t>
+  </si>
+  <si>
+    <t>abc</t>
+  </si>
+  <si>
+    <t>xyz</t>
+  </si>
+  <si>
+    <t>ABC</t>
+  </si>
+  <si>
+    <t>XYZ</t>
   </si>
 </sst>
 </file>
@@ -421,7 +443,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BB8DBD2-ED36-4C67-8A46-FC022A444717}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -450,4 +472,55 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE1D791F-64C5-4EBA-91A3-274402ECA050}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2">
+        <v>9999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3">
+        <v>8888</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>